<commit_message>
Fixed write row actions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_StagnantCarriers_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BAA17B-3542-4984-A154-510FF39E4A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD771BEE-0CCF-4607-B3FD-1EA632C12DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="795" windowWidth="21600" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -169,9 +169,6 @@
     <t>GDrive folder path where the execution reports are stored</t>
   </si>
   <si>
-    <t>GDriveMasterReport</t>
-  </si>
-  <si>
     <t>Gdrive folder path where the Master execution report is stored</t>
   </si>
   <si>
@@ -257,6 +254,18 @@
   </si>
   <si>
     <t>14_Legal_StagnantCarriers</t>
+  </si>
+  <si>
+    <t>14_GDriveMasterReportID</t>
+  </si>
+  <si>
+    <t>GDriveMasterReportPath</t>
+  </si>
+  <si>
+    <t>GDriveMasterReportID</t>
+  </si>
+  <si>
+    <t>Gdrive folder ID for the Master execution report file</t>
   </si>
 </sst>
 </file>
@@ -539,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -587,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -609,7 +618,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -620,7 +629,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -2802,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2853,7 +2862,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -2864,103 +2873,116 @@
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3975,19 +3997,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added logic to reuse the current report file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_StagnantCarriers_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD771BEE-0CCF-4607-B3FD-1EA632C12DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED455C-A131-4ECF-A461-4480AA787417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="14745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -266,6 +266,24 @@
   </si>
   <si>
     <t>Gdrive folder ID for the Master execution report file</t>
+  </si>
+  <si>
+    <t>14_ReportFileID</t>
+  </si>
+  <si>
+    <t>14_ReportFileURL</t>
+  </si>
+  <si>
+    <t>ReportFileID</t>
+  </si>
+  <si>
+    <t>ReportFileURL</t>
+  </si>
+  <si>
+    <t>Gdrive ID for the current report file</t>
+  </si>
+  <si>
+    <t>Gdrive URL for the current report file</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2830,7 @@
   <dimension ref="A1:X999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2983,8 +3001,34 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>